<commit_message>
Adding ica02 encoder / decoder + readme
</commit_message>
<xml_diff>
--- a/ica02/ICA02-Uke5-CircuitBreakers.xlsx
+++ b/ica02/ICA02-Uke5-CircuitBreakers.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndreiMac/SkyDrive/Universitate/Vår 2016/IS-105/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tor Ole\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14925" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Helse og idrettsfag</t>
   </si>
@@ -68,15 +68,29 @@
     <t>Fakultetskoder</t>
   </si>
   <si>
-    <t>Per 100 studenter</t>
+    <t>Sannsynlighet</t>
+  </si>
+  <si>
+    <t>Per 100 studenter i %</t>
+  </si>
+  <si>
+    <t>Gjennomsnitt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,8 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +130,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -383,23 +401,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -419,10 +440,10 @@
         <v>13</v>
       </c>
       <c r="P2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -447,7 +468,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -472,7 +493,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -497,7 +518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -522,7 +543,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -547,7 +568,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -572,7 +593,37 @@
         <v>28.999999999999996</v>
       </c>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <f>AVERAGE(E3:E9)</f>
+        <v>1756.5</v>
+      </c>
+      <c r="G10" s="1">
+        <f>AVERAGE(G3:G9)</f>
+        <v>16.5</v>
+      </c>
+      <c r="J10" s="1">
+        <f>AVERAGE(J3:J9)</f>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="L10" s="1">
+        <f>AVERAGE(L3:L9)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="N10" s="1">
+        <f>AVERAGE(N3:N9)</f>
+        <v>0.44666666666666671</v>
+      </c>
+      <c r="P10" s="1">
+        <f>AVERAGE(P3:P9)</f>
+        <v>44.666666666666664</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>